<commit_message>
Add of the description page, nunit description test, minor changes of the utils & the test data
</commit_message>
<xml_diff>
--- a/MarsAdvTaskNUnit/MarsAdvTaskNUnit/ExcelData/TestExcelData.xlsx
+++ b/MarsAdvTaskNUnit/MarsAdvTaskNUnit/ExcelData/TestExcelData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Other Stuff\Programming_Languages\AutomationTesting\AllProjects\ProjectMars\MarsAdvTask\MarsAdvTask\MarsAdvTaskNUnit\MarsAdvTaskNUnit\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81723539-299A-436C-9912-2B1A141FE7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F55967-EC78-4D85-8CCD-F04E70111FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -123,12 +123,6 @@
     <t>Language</t>
   </si>
   <si>
-    <t>Skills</t>
-  </si>
-  <si>
-    <t>CollegeName</t>
-  </si>
-  <si>
     <t>Level</t>
   </si>
   <si>
@@ -165,9 +159,6 @@
     <t>Fluent</t>
   </si>
   <si>
-    <t>CollegeTitle</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -330,9 +321,6 @@
     <t>Japanese</t>
   </si>
   <si>
-    <t xml:space="preserve">	Conversational</t>
-  </si>
-  <si>
     <t>JavaScript</t>
   </si>
   <si>
@@ -345,16 +333,28 @@
     <t>Japan</t>
   </si>
   <si>
-    <t>B.Tech &amp; BS</t>
-  </si>
-  <si>
-    <t>Software Testing &amp; Cloud Testing</t>
-  </si>
-  <si>
     <t>SCS</t>
   </si>
   <si>
     <t>ISTQB - CTFL</t>
+  </si>
+  <si>
+    <t>Conversational</t>
+  </si>
+  <si>
+    <t>Skill</t>
+  </si>
+  <si>
+    <t>UniversityName</t>
+  </si>
+  <si>
+    <t>UniversityTitle</t>
+  </si>
+  <si>
+    <t>Cloud Computing Testing</t>
+  </si>
+  <si>
+    <t>B.Sc</t>
   </si>
 </sst>
 </file>
@@ -712,18 +712,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -1730,7 +1730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1763,7 +1763,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -1780,7 +1780,7 @@
     </row>
     <row r="3" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1793,7 +1793,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1807,23 +1807,23 @@
         <v>30</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1837,7 +1837,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1848,10 +1848,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>31</v>
+        <v>104</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1859,15 +1859,15 @@
         <v>7</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1879,64 +1879,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4700BF2-5992-4896-BB4E-298DFF4D6E9D}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.8984375" customWidth="1"/>
+    <col min="1" max="1" width="17.09765625" customWidth="1"/>
     <col min="2" max="2" width="10.09765625" customWidth="1"/>
-    <col min="3" max="3" width="12.69921875" customWidth="1"/>
-    <col min="4" max="4" width="14.296875" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="21.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>45</v>
+        <v>106</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>92</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>95</v>
       </c>
       <c r="E2" s="15">
         <v>2022</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E3" s="15">
         <v>2021</v>
@@ -1963,32 +1963,32 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>37</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C2" s="15">
         <v>2022</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C3" s="15">
         <v>2021</v>
@@ -2031,28 +2031,28 @@
         <v>2</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>14</v>
@@ -2073,16 +2073,16 @@
         <v>11</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="R1" s="6" t="s">
         <v>13</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="11" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
@@ -2093,19 +2093,19 @@
         <v>18</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>19</v>
@@ -2135,36 +2135,36 @@
         <v>19</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="R2" s="11">
         <v>10</v>
       </c>
       <c r="S2" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="11" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>83</v>
-      </c>
       <c r="E3" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>7</v>
@@ -2194,13 +2194,13 @@
         <v>21</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="R3" s="11">
         <v>7</v>
       </c>
       <c r="S3" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="11" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
@@ -2208,22 +2208,22 @@
         <v>23</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>25</v>
@@ -2250,7 +2250,7 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>12</v>
@@ -2259,18 +2259,18 @@
         <v>5</v>
       </c>
       <c r="S4" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>88</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>91</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>15</v>
@@ -2285,7 +2285,7 @@
         <v>44946</v>
       </c>
       <c r="P5" s="11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -2339,35 +2339,35 @@
         <v>14</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>22</v>
@@ -2376,7 +2376,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>23</v>
@@ -2391,13 +2391,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>22</v>
@@ -2406,13 +2406,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>15</v>
@@ -2441,42 +2441,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="E1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated of the Excel Data & reports
</commit_message>
<xml_diff>
--- a/MarsAdvTaskNUnit/MarsAdvTaskNUnit/ExcelData/TestExcelData.xlsx
+++ b/MarsAdvTaskNUnit/MarsAdvTaskNUnit/ExcelData/TestExcelData.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Other Stuff\Programming_Languages\AutomationTesting\AllProjects\ProjectMars\MarsAdvTask\MarsAdvTask\MarsAdvTaskNUnit\MarsAdvTaskNUnit\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F55967-EC78-4D85-8CCD-F04E70111FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D196DB5-A74E-4780-9AB1-72F72B1F2C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="ProfileDescription" sheetId="3" r:id="rId2"/>
     <sheet name="ProfileLanguage" sheetId="6" r:id="rId3"/>
-    <sheet name="ProfileSkills" sheetId="9" r:id="rId4"/>
+    <sheet name="ProfileSkill" sheetId="9" r:id="rId4"/>
     <sheet name="ProfileEducation" sheetId="7" r:id="rId5"/>
-    <sheet name="ProfileCertifications" sheetId="8" r:id="rId6"/>
+    <sheet name="ProfileCertification" sheetId="8" r:id="rId6"/>
     <sheet name="ShareSkill" sheetId="2" r:id="rId7"/>
     <sheet name="ManageListings" sheetId="4" r:id="rId8"/>
     <sheet name="Register" sheetId="5" r:id="rId9"/>
@@ -138,9 +138,6 @@
     <t>Certificate</t>
   </si>
   <si>
-    <t>From</t>
-  </si>
-  <si>
     <t>CertificationYear</t>
   </si>
   <si>
@@ -355,6 +352,9 @@
   </si>
   <si>
     <t>B.Sc</t>
+  </si>
+  <si>
+    <t>CertificateFrom</t>
   </si>
 </sst>
 </file>
@@ -712,18 +712,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -1763,7 +1763,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -1780,7 +1780,7 @@
     </row>
     <row r="3" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1812,18 +1812,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1848,7 +1848,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>32</v>
@@ -1859,15 +1859,15 @@
         <v>7</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>97</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1879,7 +1879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4700BF2-5992-4896-BB4E-298DFF4D6E9D}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -1893,16 +1893,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>33</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>34</v>
@@ -1910,16 +1910,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>90</v>
-      </c>
       <c r="C2" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E2" s="15">
         <v>2022</v>
@@ -1927,16 +1927,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>100</v>
-      </c>
       <c r="C3" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E3" s="15">
         <v>2021</v>
@@ -1951,13 +1951,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02FD410F-AE87-4FF1-AA7A-A06EA9F2CE8F}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.296875" customWidth="1"/>
+    <col min="1" max="1" width="14.8984375" customWidth="1"/>
+    <col min="2" max="2" width="19.59765625" customWidth="1"/>
     <col min="3" max="3" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1966,18 +1967,18 @@
         <v>35</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2" s="15">
         <v>2022</v>
@@ -1985,10 +1986,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C3" s="15">
         <v>2021</v>
@@ -2031,28 +2032,28 @@
         <v>2</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>70</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>14</v>
@@ -2073,16 +2074,16 @@
         <v>11</v>
       </c>
       <c r="P1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q1" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>72</v>
       </c>
       <c r="R1" s="6" t="s">
         <v>13</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="11" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
@@ -2093,19 +2094,19 @@
         <v>18</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>19</v>
@@ -2135,36 +2136,36 @@
         <v>19</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R2" s="11">
         <v>10</v>
       </c>
       <c r="S2" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="11" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>59</v>
-      </c>
       <c r="C3" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>7</v>
@@ -2194,13 +2195,13 @@
         <v>21</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R3" s="11">
         <v>7</v>
       </c>
       <c r="S3" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="11" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
@@ -2208,22 +2209,22 @@
         <v>23</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>25</v>
@@ -2250,7 +2251,7 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>12</v>
@@ -2259,18 +2260,18 @@
         <v>5</v>
       </c>
       <c r="S4" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>86</v>
-      </c>
       <c r="H5" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>15</v>
@@ -2285,7 +2286,7 @@
         <v>44946</v>
       </c>
       <c r="P5" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -2339,35 +2340,35 @@
         <v>14</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>59</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>22</v>
@@ -2376,7 +2377,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>23</v>
@@ -2391,13 +2392,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>22</v>
@@ -2406,13 +2407,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>15</v>
@@ -2441,42 +2442,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" t="s">
-        <v>48</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>52</v>
-      </c>
       <c r="E2" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added of the share skill page & share skill of nunit test
</commit_message>
<xml_diff>
--- a/MarsAdvTaskNUnit/MarsAdvTaskNUnit/ExcelData/TestExcelData.xlsx
+++ b/MarsAdvTaskNUnit/MarsAdvTaskNUnit/ExcelData/TestExcelData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Other Stuff\Programming_Languages\AutomationTesting\AllProjects\ProjectMars\MarsAdvTask\MarsAdvTask\MarsAdvTaskNUnit\MarsAdvTaskNUnit\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D196DB5-A74E-4780-9AB1-72F72B1F2C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C93582F-B786-4E64-B4EC-51A9DBB486D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -21,14 +21,15 @@
     <sheet name="ProfileCertification" sheetId="8" r:id="rId6"/>
     <sheet name="ShareSkill" sheetId="2" r:id="rId7"/>
     <sheet name="ManageListings" sheetId="4" r:id="rId8"/>
-    <sheet name="Register" sheetId="5" r:id="rId9"/>
+    <sheet name="SearchSkill" sheetId="10" r:id="rId9"/>
+    <sheet name="Register" sheetId="5" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="111">
   <si>
     <t>username</t>
   </si>
@@ -355,6 +356,12 @@
   </si>
   <si>
     <t>CertificateFrom</t>
+  </si>
+  <si>
+    <t>SearchCategory</t>
+  </si>
+  <si>
+    <t>Fun &amp; Lifestyle</t>
   </si>
 </sst>
 </file>
@@ -435,7 +442,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -475,6 +482,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1726,6 +1734,71 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="23.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.69921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" display="Mayuri@123" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" display="Mayuri@123" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M3"/>
@@ -1951,7 +2024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02FD410F-AE87-4FF1-AA7A-A06EA9F2CE8F}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -2004,8 +2077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2121,10 +2194,10 @@
         <v>17</v>
       </c>
       <c r="L2" s="12">
-        <v>44545</v>
+        <v>44910</v>
       </c>
       <c r="M2" s="12">
-        <v>44910</v>
+        <v>45275</v>
       </c>
       <c r="N2" s="13">
         <v>0.39583333333333331</v>
@@ -2180,10 +2253,10 @@
         <v>29</v>
       </c>
       <c r="L3" s="12">
-        <v>44552</v>
+        <v>44917</v>
       </c>
       <c r="M3" s="12">
-        <v>44917</v>
+        <v>45282</v>
       </c>
       <c r="N3" s="13">
         <v>0.41666666666666669</v>
@@ -2239,10 +2312,10 @@
         <v>29</v>
       </c>
       <c r="L4" s="12">
-        <v>44555</v>
+        <v>44920</v>
       </c>
       <c r="M4" s="12">
-        <v>44920</v>
+        <v>45285</v>
       </c>
       <c r="N4" s="13">
         <v>0.5</v>
@@ -2280,10 +2353,10 @@
         <v>17</v>
       </c>
       <c r="L5" s="12">
-        <v>44581</v>
+        <v>44793</v>
       </c>
       <c r="M5" s="12">
-        <v>44946</v>
+        <v>45158</v>
       </c>
       <c r="P5" s="11" t="s">
         <v>86</v>
@@ -2426,66 +2499,29 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871C730D-680C-4BA0-ACCF-F2FEBE7A69AA}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="23.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>48</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" display="Mayuri@123" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" display="Mayuri@123" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Minor changes of the files
</commit_message>
<xml_diff>
--- a/MarsAdvTaskNUnit/MarsAdvTaskNUnit/ExcelData/TestExcelData.xlsx
+++ b/MarsAdvTaskNUnit/MarsAdvTaskNUnit/ExcelData/TestExcelData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Other Stuff\Programming_Languages\AutomationTesting\AllProjects\ProjectMars\MarsAdvTask\MarsAdvTask\MarsAdvTaskNUnit\MarsAdvTaskNUnit\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C93582F-B786-4E64-B4EC-51A9DBB486D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D0AD84-59F7-4391-A3A8-07ED7A5949B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="117">
   <si>
     <t>username</t>
   </si>
@@ -361,7 +361,25 @@
     <t>SearchCategory</t>
   </si>
   <si>
-    <t>Fun &amp; Lifestyle</t>
+    <t>Music &amp; Audio</t>
+  </si>
+  <si>
+    <t>manalijain167@gmail.com</t>
+  </si>
+  <si>
+    <t>Manali</t>
+  </si>
+  <si>
+    <t>Testing123</t>
+  </si>
+  <si>
+    <t>sravankumar670@gmail.com</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t>Sample120</t>
   </si>
 </sst>
 </file>
@@ -372,7 +390,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="[$-10409]h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,11 +405,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <u/>
@@ -437,34 +450,33 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -473,13 +485,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -702,7 +714,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -719,27 +731,42 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
+    <row r="3" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
@@ -1728,9 +1755,12 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="Mayuri@123" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{E1A5AEEE-43D8-487F-9B2F-B526B00EC863}"/>
+    <hyperlink ref="B3" r:id="rId4" display="Mayuri@123" xr:uid="{4FB967C8-D94C-49B4-9737-F74648201376}"/>
+    <hyperlink ref="A4" r:id="rId5" xr:uid="{9226B856-4D27-40BF-8A79-DC71958035C2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -1750,7 +1780,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B1" t="s">
@@ -1765,27 +1795,27 @@
       <c r="E1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1818,41 +1848,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="15"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1876,26 +1906,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1920,26 +1950,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1965,53 +1995,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="14">
         <v>2022</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="14">
         <v>2021</v>
       </c>
     </row>
@@ -2036,35 +2066,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="14">
         <v>2022</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="14">
         <v>2021</v>
       </c>
     </row>
@@ -2077,8 +2107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2100,281 +2130,281 @@
     <col min="19" max="19" width="10.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="S1" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="11" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:19" s="10" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="12">
+      <c r="L2" s="11">
         <v>44910</v>
       </c>
-      <c r="M2" s="12">
+      <c r="M2" s="11">
         <v>45275</v>
       </c>
-      <c r="N2" s="13">
+      <c r="N2" s="12">
         <v>0.39583333333333331</v>
       </c>
-      <c r="O2" s="13">
+      <c r="O2" s="12">
         <v>0.70833333333333337</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="Q2" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="R2" s="11">
+      <c r="R2" s="10">
         <v>10</v>
       </c>
-      <c r="S2" s="11" t="s">
+      <c r="S2" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="11" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:19" s="10" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="11">
         <v>44917</v>
       </c>
-      <c r="M3" s="12">
+      <c r="M3" s="11">
         <v>45282</v>
       </c>
-      <c r="N3" s="13">
+      <c r="N3" s="12">
         <v>0.41666666666666669</v>
       </c>
-      <c r="O3" s="13">
+      <c r="O3" s="12">
         <v>0.72916666666666663</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="R3" s="11">
+      <c r="R3" s="10">
         <v>7</v>
       </c>
-      <c r="S3" s="11" t="s">
+      <c r="S3" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="11" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:19" s="10" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="11">
         <v>44920</v>
       </c>
-      <c r="M4" s="12">
+      <c r="M4" s="11">
         <v>45285</v>
       </c>
-      <c r="N4" s="13">
+      <c r="N4" s="12">
         <v>0.5</v>
       </c>
-      <c r="O4" s="13">
+      <c r="O4" s="12">
         <v>0.77083333333333337</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="P4" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="Q4" s="6" t="s">
+      <c r="Q4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="R4" s="11">
+      <c r="R4" s="10">
         <v>5</v>
       </c>
-      <c r="S4" s="11" t="s">
+      <c r="S4" s="10" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="11">
         <v>44793</v>
       </c>
-      <c r="M5" s="12">
+      <c r="M5" s="11">
         <v>45158</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="P5" s="10" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="H6" s="7"/>
-      <c r="I6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="7"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="9"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2400,98 +2430,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="11"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="11"/>
+      <c r="E6" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2500,25 +2530,30 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871C730D-680C-4BA0-ACCF-F2FEBE7A69AA}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>